<commit_message>
handle excel data;test works
</commit_message>
<xml_diff>
--- a/data/SchoolData.xlsx
+++ b/data/SchoolData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t xml:space="preserve">MONDAY</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t xml:space="preserve">Room C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StudentGroup</t>
   </si>
   <si>
     <t xml:space="preserve">Math</t>
@@ -122,6 +131,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,6 +152,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,9 +237,9 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
   </cols>
   <sheetData>
@@ -418,7 +429,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -460,18 +471,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.48"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
@@ -481,30 +492,30 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -513,152 +524,152 @@
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -667,91 +678,105 @@
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel parser fix: empty strings to nulls
</commit_message>
<xml_diff>
--- a/data/SchoolData.xlsx
+++ b/data/SchoolData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t xml:space="preserve">MONDAY</t>
   </si>
@@ -58,15 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">Room C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teacher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StudentGroup</t>
   </si>
   <si>
     <t xml:space="preserve">Math</t>
@@ -237,9 +228,9 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
   </cols>
   <sheetData>
@@ -429,7 +420,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -471,18 +462,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.48"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
@@ -492,30 +486,30 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -524,152 +518,152 @@
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -678,105 +672,91 @@
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Download school example xlsx file web endpoint.
</commit_message>
<xml_diff>
--- a/data/SchoolData.xlsx
+++ b/data/SchoolData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="timeslotList" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,10 +33,10 @@
     <t xml:space="preserve">09:30:00</t>
   </si>
   <si>
+    <t xml:space="preserve">10:30:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">11:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">13:30:00</t>
@@ -224,13 +224,13 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
   </cols>
   <sheetData>
@@ -270,10 +270,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,10 +340,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,7 +420,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -464,14 +464,11 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.48"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -675,12 +672,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>

</xml_diff>